<commit_message>
latest update- add calories of items
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\aliki\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\aliki-menu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0036A005-F73A-4C85-A633-9C601D1964AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA18A82-92BB-4161-8FDD-946F8D0B6EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4CC42C16-0820-4E66-B67B-FAAD95487B1B}"/>
+    <workbookView xWindow="9915" yWindow="-375" windowWidth="15375" windowHeight="8655" firstSheet="4" activeTab="6" xr2:uid="{4CC42C16-0820-4E66-B67B-FAAD95487B1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_Hlk111376100" localSheetId="0">Sheet1!$B$3</definedName>
-    <definedName name="_Hlk111461294" localSheetId="0">Sheet1!$C$33</definedName>
+    <definedName name="_Hlk111461294" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="95">
   <si>
     <t xml:space="preserve">Crispy chicken bites </t>
   </si>
@@ -67,9 +68,6 @@
     <t>Mac &amp; Cheese  Ball</t>
   </si>
   <si>
-    <t>f8.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chicken Lollipop </t>
   </si>
   <si>
@@ -94,24 +92,6 @@
     <t>Fried herb panko crumbed mozzarella pop with maple mayo.</t>
   </si>
   <si>
-    <t>f5.png</t>
-  </si>
-  <si>
-    <t>f6.png</t>
-  </si>
-  <si>
-    <t>f2.png</t>
-  </si>
-  <si>
-    <t>f4.png</t>
-  </si>
-  <si>
-    <t>f7.png</t>
-  </si>
-  <si>
-    <t>Salads</t>
-  </si>
-  <si>
     <t>Beet salad with spinach</t>
   </si>
   <si>
@@ -130,9 +110,6 @@
     <t>Caesar dressing romaine lettuce,  grilled chicken, beef bacon, herb croutons &amp; grated parmesan.</t>
   </si>
   <si>
-    <t>Fries</t>
-  </si>
-  <si>
     <t>Dynamite fries</t>
   </si>
   <si>
@@ -148,9 +125,6 @@
     <t>Regular fries</t>
   </si>
   <si>
-    <t>BEEF BURGERS</t>
-  </si>
-  <si>
     <t>Cheeseburger</t>
   </si>
   <si>
@@ -169,9 +143,6 @@
     <t>Our homemade special Angus beef patty, cheddar, grilled mushrooms, jalapeno, bacon jam &amp; creamy Italian cheese, and red beetroot Seamen bun.</t>
   </si>
   <si>
-    <t>Chicken Burgers</t>
-  </si>
-  <si>
     <t>Classical fried chicken burger (Fried)</t>
   </si>
   <si>
@@ -214,24 +185,6 @@
     <t>Grilled beef sausage, crispy fried onion rings, cheese, lettuce with mustard &amp; tomato sauce, mayo, and potato bun.</t>
   </si>
   <si>
-    <t>BEEF HOT DOGS</t>
-  </si>
-  <si>
-    <t>Sandwich</t>
-  </si>
-  <si>
-    <t>Philly Beef Steak Sandwich</t>
-  </si>
-  <si>
-    <t>Thinly sliced Angus beef, grilled with onion, bell pepper topped with B.B.Q mayo &amp; English cheddar melt, and potato bun.</t>
-  </si>
-  <si>
-    <t>Philly chicken cheese steak Sandwich</t>
-  </si>
-  <si>
-    <t>slice chicken breast, grilled mushroom, cooked with cream cheese, and potato bun.</t>
-  </si>
-  <si>
     <t>Grilled con, coated with creamy Mexican sauce.</t>
   </si>
   <si>
@@ -317,6 +270,66 @@
   </si>
   <si>
     <t>Split_burger__Grilled.png</t>
+  </si>
+  <si>
+    <t>drinks</t>
+  </si>
+  <si>
+    <t>cal</t>
+  </si>
+  <si>
+    <t>Aliki Lemonade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passtionfruit mojito </t>
+  </si>
+  <si>
+    <t>Blue Mojito</t>
+  </si>
+  <si>
+    <t>Strawberry mojito</t>
+  </si>
+  <si>
+    <t>Blueberry lemonade</t>
+  </si>
+  <si>
+    <t>Ice tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodas drinks </t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Blue Mojito.png</t>
+  </si>
+  <si>
+    <t>Blueberry lemonade.png</t>
+  </si>
+  <si>
+    <t>Passtionfruit mojito.png</t>
+  </si>
+  <si>
+    <t>peps.png</t>
+  </si>
+  <si>
+    <t>Strawberry mojito.png</t>
+  </si>
+  <si>
+    <t>water.png</t>
+  </si>
+  <si>
+    <t>ليموناد اليكي الخاص.png</t>
+  </si>
+  <si>
+    <t>Ice tea.png</t>
+  </si>
+  <si>
+    <t>classic burgur</t>
+  </si>
+  <si>
+    <t>double Cheeseburger</t>
   </si>
 </sst>
 </file>
@@ -332,7 +345,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,18 +364,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -376,15 +377,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +701,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +717,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
@@ -744,22 +743,22 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -770,19 +769,19 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -793,19 +792,19 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -832,553 +831,27 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>29</v>
-      </c>
-      <c r="C11">
-        <v>29</v>
-      </c>
-      <c r="D11">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3">
-        <v>3</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17">
-        <v>29</v>
-      </c>
-      <c r="C17">
-        <v>29</v>
-      </c>
-      <c r="D17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22">
-        <v>30</v>
-      </c>
-      <c r="C22">
-        <v>34</v>
-      </c>
-      <c r="D22">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3">
-        <v>2</v>
-      </c>
-      <c r="D25" s="3">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3">
-        <v>4</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
-      <c r="G25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28">
-        <v>26</v>
-      </c>
-      <c r="C28">
-        <v>27</v>
-      </c>
-      <c r="D28">
-        <v>27</v>
-      </c>
-      <c r="E28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
-        <v>2</v>
-      </c>
-      <c r="D31" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34">
-        <v>25</v>
-      </c>
-      <c r="C34">
-        <v>23</v>
-      </c>
-      <c r="D34">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="3">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3">
-        <v>2</v>
-      </c>
-      <c r="D37" s="3">
-        <v>3</v>
-      </c>
-      <c r="E37" s="3">
-        <v>4</v>
-      </c>
-      <c r="F37" s="3">
-        <v>5</v>
-      </c>
-      <c r="G37" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" t="s">
-        <v>61</v>
-      </c>
-      <c r="D39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40">
-        <v>30</v>
-      </c>
-      <c r="C40">
-        <v>30</v>
-      </c>
-      <c r="D40">
-        <v>32</v>
-      </c>
-      <c r="E40">
-        <v>24</v>
-      </c>
-      <c r="F40">
-        <v>24</v>
-      </c>
-      <c r="G40">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="A6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>370</v>
+      </c>
+      <c r="C6">
+        <v>350</v>
+      </c>
+      <c r="D6">
+        <v>420</v>
+      </c>
+      <c r="E6">
+        <v>450</v>
+      </c>
+      <c r="F6">
+        <v>220</v>
+      </c>
+      <c r="G6">
+        <v>480</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
@@ -1397,17 +870,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D58A7C-6858-4EEF-8057-5F7B01A12E6B}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B1" s="3">
         <v>2</v>
@@ -1424,13 +897,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,13 +911,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1452,13 +925,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,6 +946,20 @@
       </c>
       <c r="D5">
         <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>280</v>
+      </c>
+      <c r="C6">
+        <v>210</v>
+      </c>
+      <c r="D6">
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -1482,17 +969,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443A965E-7A36-41CA-AE04-04BEE90C6230}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
@@ -1509,13 +996,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1523,13 +1010,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1537,13 +1024,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1558,6 +1045,20 @@
       </c>
       <c r="D5">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>380</v>
+      </c>
+      <c r="C6">
+        <v>380</v>
+      </c>
+      <c r="D6">
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -1567,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1F980C-8AFF-4F99-8BA1-59869F2E6632}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,7 +1081,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3">
         <v>3</v>
@@ -1597,13 +1098,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1611,13 +1112,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1625,13 +1126,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1646,6 +1147,36 @@
       </c>
       <c r="D5">
         <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>610</v>
+      </c>
+      <c r="C6">
+        <v>810</v>
+      </c>
+      <c r="D6">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9">
+        <v>860</v>
       </c>
     </row>
   </sheetData>
@@ -1655,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70172219-E402-445A-AF5F-B88FB20D0E15}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A6" sqref="A6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,7 +1199,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
@@ -1688,16 +1219,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1705,16 +1236,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1722,16 +1253,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1749,6 +1280,23 @@
       </c>
       <c r="E5">
         <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>680</v>
+      </c>
+      <c r="C6">
+        <v>460</v>
+      </c>
+      <c r="D6">
+        <v>840</v>
+      </c>
+      <c r="E6">
+        <v>880</v>
       </c>
     </row>
   </sheetData>
@@ -1757,11 +1305,110 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA29EB2-7651-491F-B4A3-F676B0A20A6D}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55043A55-A1A3-40EA-8940-DC6BFFC69F89}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>840</v>
+      </c>
+      <c r="C6">
+        <v>830</v>
+      </c>
+      <c r="D6">
+        <v>680</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA29EB2-7651-491F-B4A3-F676B0A20A6D}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,9 +1416,9 @@
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
@@ -1782,64 +1429,136 @@
       <c r="D1" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="E3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>250</v>
+      </c>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6">
+        <v>320</v>
+      </c>
+      <c r="E6">
+        <v>600</v>
+      </c>
+      <c r="F6">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new image for foods
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\aliki-menu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA18A82-92BB-4161-8FDD-946F8D0B6EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF8E808-0AA3-468D-8190-1F057007B8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9915" yWindow="-375" windowWidth="15375" windowHeight="8655" firstSheet="4" activeTab="6" xr2:uid="{4CC42C16-0820-4E66-B67B-FAAD95487B1B}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="8655" firstSheet="4" activeTab="6" xr2:uid="{4CC42C16-0820-4E66-B67B-FAAD95487B1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1408,7 +1408,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,7 +1542,7 @@
         <v>76</v>
       </c>
       <c r="B6">
-        <v>250</v>
+        <v>460</v>
       </c>
       <c r="C6">
         <v>300</v>
@@ -1555,6 +1555,9 @@
       </c>
       <c r="F6">
         <v>320</v>
+      </c>
+      <c r="I6">
+        <v>710</v>
       </c>
     </row>
   </sheetData>

</xml_diff>